<commit_message>
Reevz last day on earth
</commit_message>
<xml_diff>
--- a/Order_History.xlsx
+++ b/Order_History.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,79 +429,70 @@
         <v>Tax (₹)</v>
       </c>
       <c r="I1" t="str">
-        <v>Reason</v>
-      </c>
-      <c r="J1" t="str">
         <v>Food Items</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1">
-        <v>45686.22928240741</v>
+        <v>45691.22928240741</v>
       </c>
       <c r="C2" t="str">
-        <v>Notsla Daniel</v>
+        <v>Reevan</v>
       </c>
       <c r="D2">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="E2">
-        <v>490</v>
+        <v>429</v>
       </c>
       <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2">
         <v>2</v>
       </c>
-      <c r="G2">
-        <v>6</v>
-      </c>
       <c r="H2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I2" t="str">
-        <v>Vegetarian got meat in the mouth</v>
-      </c>
-      <c r="J2" t="str">
-        <v>Coffee Italia (x3)</v>
+        <v>Vanilla Shake (x2)</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>121</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>45679.22928240741</v>
+        <v>45686.22928240741</v>
       </c>
       <c r="C3" t="str">
-        <v>Ajay Francis Anchan</v>
+        <v>Karthik</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>123</v>
+        <v>790</v>
       </c>
       <c r="F3">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H3">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="I3" t="str">
-        <v>Third year gave the wrong order</v>
-      </c>
-      <c r="J3" t="str">
-        <v>Veg Cheese Pops (x2)</v>
+        <v>Vanilla Shake (x4), Mango Lassi (x2)</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>